<commit_message>
Adding files into GIT
</commit_message>
<xml_diff>
--- a/Resources/DemoQAFormData.xlsx
+++ b/Resources/DemoQAFormData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ranjith\Learnings\Projects\RobotProject\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C963A8-75CB-4AB5-ACF1-6E02294A01B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B844DA0-2A33-4CC3-8124-EE652444E412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{050D9092-A045-488A-8874-2452B857ACC6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{050D9092-A045-488A-8874-2452B857ACC6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
   <si>
     <t>FIRST_NAME</t>
   </si>
@@ -86,17 +86,95 @@
     <t>SAIDAPET, CHENNAI</t>
   </si>
   <si>
-    <t>TAMILNADU</t>
-  </si>
-  <si>
-    <t>CHENNAI</t>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>Haryana</t>
+  </si>
+  <si>
+    <t>Panipat</t>
+  </si>
+  <si>
+    <t>Karthick</t>
+  </si>
+  <si>
+    <t>Saranya</t>
+  </si>
+  <si>
+    <t>Parthiban</t>
+  </si>
+  <si>
+    <t>Ashwini</t>
+  </si>
+  <si>
+    <t>Santhosh</t>
+  </si>
+  <si>
+    <t>Sankaran</t>
+  </si>
+  <si>
+    <t>Patel</t>
+  </si>
+  <si>
+    <t>karthick@gmail.com</t>
+  </si>
+  <si>
+    <t>ranjith@gmail.com</t>
+  </si>
+  <si>
+    <t>saransant@gmail.com</t>
+  </si>
+  <si>
+    <t>parthiban@gmail.com</t>
+  </si>
+  <si>
+    <t>ashpat@gmail.com</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>MATHS, PHYSICS</t>
+  </si>
+  <si>
+    <t>TAMIL, MATHS</t>
+  </si>
+  <si>
+    <t>ENGLISH, PHYSICS</t>
+  </si>
+  <si>
+    <t>TAMIL, ENGLISH, MATHS, PHYSICS</t>
+  </si>
+  <si>
+    <t>SPORTS</t>
+  </si>
+  <si>
+    <t>READING, MUSIC</t>
+  </si>
+  <si>
+    <t>RADING</t>
+  </si>
+  <si>
+    <t>MUSIC</t>
+  </si>
+  <si>
+    <t>GUINDY, CHENNAI</t>
+  </si>
+  <si>
+    <t>BANGLORE</t>
+  </si>
+  <si>
+    <t>SALEM</t>
+  </si>
+  <si>
+    <t>PANIPAT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,6 +187,14 @@
       <color rgb="FF871094"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -128,17 +214,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -451,28 +540,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64341086-7E0F-4035-84EB-C406928AE7BB}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.90625" customWidth="1"/>
     <col min="2" max="2" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -480,98 +570,262 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="D2">
-        <v>9884886760</v>
-      </c>
-      <c r="E2" s="2">
-        <v>31229</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="E2">
+        <v>9876543210</v>
+      </c>
+      <c r="F2" s="2">
+        <v>32880</v>
+      </c>
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>15</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
       </c>
       <c r="J2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="K2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3">
+        <v>9876543210</v>
+      </c>
+      <c r="F3" s="2">
+        <v>33277</v>
+      </c>
+      <c r="G3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4">
+        <v>9876543210</v>
+      </c>
+      <c r="F4" s="2">
+        <v>33672</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5">
+        <v>9876543210</v>
+      </c>
+      <c r="F5" s="2">
+        <v>34069</v>
+      </c>
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6">
+        <v>9876543210</v>
+      </c>
+      <c r="F6" s="2">
+        <v>34465</v>
+      </c>
+      <c r="G6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:12">
       <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:12">
       <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:12">
       <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:12">
       <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:12">
       <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:12">
       <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:12">
       <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:12">
       <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="2:2">
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="2:3">
       <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="2:2">
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="2:3">
       <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{E9C11DCC-2B40-470C-8A25-6C5BD1307D1B}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{FF626E07-8DA6-4065-80DB-FB0789059305}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{84EFCE06-B4E1-4703-BFDD-110B83CBB3C5}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{5CA92B60-A7D9-47F1-BF6F-8C8A07AC1AB3}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{4B41CD06-194E-47D5-8AEF-521688966EA9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the changes and push to GIT
</commit_message>
<xml_diff>
--- a/Resources/DemoQAFormData.xlsx
+++ b/Resources/DemoQAFormData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ranjith\Learnings\Projects\RobotProject\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B844DA0-2A33-4CC3-8124-EE652444E412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9F2E58-68FC-46F8-AD1A-766F230A2E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{050D9092-A045-488A-8874-2452B857ACC6}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{050D9092-A045-488A-8874-2452B857ACC6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="PersonDetails" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="45">
   <si>
     <t>FIRST_NAME</t>
   </si>
@@ -168,6 +169,9 @@
   </si>
   <si>
     <t>PANIPAT</t>
+  </si>
+  <si>
+    <t>USER_ID</t>
   </si>
 </sst>
 </file>
@@ -540,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64341086-7E0F-4035-84EB-C406928AE7BB}">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -553,16 +557,9 @@
     <col min="3" max="3" width="14.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -578,27 +575,8 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1"/>
-    </row>
-    <row r="2" spans="1:12">
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -614,26 +592,8 @@
       <c r="E2">
         <v>9876543210</v>
       </c>
-      <c r="F2" s="2">
-        <v>32880</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -649,26 +609,8 @@
       <c r="E3">
         <v>9876543210</v>
       </c>
-      <c r="F3" s="2">
-        <v>33277</v>
-      </c>
-      <c r="G3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -684,26 +626,8 @@
       <c r="E4">
         <v>9876543210</v>
       </c>
-      <c r="F4" s="2">
-        <v>33672</v>
-      </c>
-      <c r="G4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I4" t="s">
-        <v>41</v>
-      </c>
-      <c r="J4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -719,26 +643,8 @@
       <c r="E5">
         <v>9876543210</v>
       </c>
-      <c r="F5" s="2">
-        <v>34069</v>
-      </c>
-      <c r="G5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" t="s">
-        <v>39</v>
-      </c>
-      <c r="I5" t="s">
-        <v>42</v>
-      </c>
-      <c r="J5" t="s">
-        <v>17</v>
-      </c>
-      <c r="K5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -754,58 +660,40 @@
       <c r="E6">
         <v>9876543210</v>
       </c>
-      <c r="F6" s="2">
-        <v>34465</v>
-      </c>
-      <c r="G6" t="s">
-        <v>35</v>
-      </c>
-      <c r="H6" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" t="s">
-        <v>43</v>
-      </c>
-      <c r="J6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+    </row>
+    <row r="8" spans="1:5">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:5">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:5">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:5">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:5">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:5">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:5">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:5">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:5">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
@@ -828,4 +716,313 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A634DE41-BB7B-45DC-87A6-C7A1B07CF309}">
+  <dimension ref="A1:M18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="2" max="2" width="12.90625" customWidth="1"/>
+    <col min="3" max="3" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2">
+        <v>1001</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2">
+        <v>9876543210</v>
+      </c>
+      <c r="G2" s="2">
+        <v>32880</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3">
+        <v>1002</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3">
+        <v>9876543210</v>
+      </c>
+      <c r="G3" s="2">
+        <v>33277</v>
+      </c>
+      <c r="H3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4">
+        <v>1003</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4">
+        <v>9876543210</v>
+      </c>
+      <c r="G4" s="2">
+        <v>33672</v>
+      </c>
+      <c r="H4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5">
+        <v>1004</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5">
+        <v>9876543210</v>
+      </c>
+      <c r="G5" s="2">
+        <v>34069</v>
+      </c>
+      <c r="H5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6">
+        <v>1005</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6">
+        <v>9876543210</v>
+      </c>
+      <c r="G6" s="2">
+        <v>34465</v>
+      </c>
+      <c r="H6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="3:4">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="3:4">
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{91B2E93F-21E1-4C07-90FD-E4259F30309D}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{D54F3883-866E-49D1-93D1-DD6A8B468D16}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{B7EC40DF-7E83-4C8B-A4BA-30F5C4A0D390}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{3040AC74-0B9D-41B1-AA52-91BE2B1F6825}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{C5454052-4E2A-48A2-968B-235730398ABE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
+</worksheet>
 </file>
</xml_diff>